<commit_message>
Fixed some stuff with loading
</commit_message>
<xml_diff>
--- a/Sample_graph.xlsx
+++ b/Sample_graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6855" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6855" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Vertices" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -457,15 +457,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated data for sample graph
</commit_message>
<xml_diff>
--- a/Sample_graph.xlsx
+++ b/Sample_graph.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/00b60d3bafc02968/Documents/Independent Study/Graph processing system/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documents\Independent Study\Graph processing system\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6855" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6855" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vertices" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -455,15 +455,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,6 +538,78 @@
       </c>
       <c r="B10">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>